<commit_message>
latest changes, reaction SBOTerm
</commit_message>
<xml_diff>
--- a/sbmlutils/examples/models/tiny_model/annotations.xlsx
+++ b/sbmlutils/examples/models/tiny_model/annotations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="106">
   <si>
     <t xml:space="preserve">pattern</t>
   </si>
@@ -266,6 +266,36 @@
   </si>
   <si>
     <t xml:space="preserve">+1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEBI:43474</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hydrogenphosphate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C00009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HO4P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h2o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEBI:15377</t>
+  </si>
+  <si>
+    <t xml:space="preserve">water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C00001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2O</t>
   </si>
   <si>
     <t xml:space="preserve"># reactions</t>
@@ -566,22 +596,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+      <selection pane="topLeft" activeCell="F62" activeCellId="0" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="19.1428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.5867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.9438775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.1428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="32.6938775510204"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="1" width="19.1428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="19.1428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="19.5357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.3571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.1632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.4030612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.5357142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="33.5765306122449"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="1" width="19.5357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="19.5357142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -606,6 +636,10 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -617,6 +651,10 @@
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7"/>
@@ -638,6 +676,10 @@
       <c r="G3" s="11" t="s">
         <v>13</v>
       </c>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
@@ -661,6 +703,10 @@
       <c r="G4" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
@@ -684,6 +730,10 @@
       <c r="G5" s="11" t="s">
         <v>21</v>
       </c>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -695,6 +745,10 @@
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
       <c r="G6" s="5"/>
+      <c r="H6" s="0"/>
+      <c r="I6" s="0"/>
+      <c r="J6" s="0"/>
+      <c r="K6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
@@ -718,6 +772,10 @@
       <c r="G7" s="11" t="s">
         <v>27</v>
       </c>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
@@ -741,6 +799,10 @@
       <c r="G8" s="11" t="s">
         <v>29</v>
       </c>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
@@ -764,6 +826,10 @@
       <c r="G9" s="11" t="s">
         <v>29</v>
       </c>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
+      <c r="J9" s="0"/>
+      <c r="K9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
@@ -773,6 +839,10 @@
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
+      <c r="H10" s="0"/>
+      <c r="I10" s="0"/>
+      <c r="J10" s="0"/>
+      <c r="K10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
@@ -784,6 +854,10 @@
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
       <c r="G11" s="5"/>
+      <c r="H11" s="0"/>
+      <c r="I11" s="0"/>
+      <c r="J11" s="0"/>
+      <c r="K11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
@@ -807,6 +881,10 @@
       <c r="G12" s="11" t="s">
         <v>36</v>
       </c>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0"/>
+      <c r="J12" s="0"/>
+      <c r="K12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
@@ -830,6 +908,10 @@
       <c r="G13" s="11" t="s">
         <v>39</v>
       </c>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13"/>
@@ -839,6 +921,10 @@
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
+      <c r="H14" s="0"/>
+      <c r="I14" s="0"/>
+      <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
@@ -850,6 +936,10 @@
       <c r="E15" s="5"/>
       <c r="F15" s="6"/>
       <c r="G15" s="5"/>
+      <c r="H15" s="0"/>
+      <c r="I15" s="0"/>
+      <c r="J15" s="0"/>
+      <c r="K15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
@@ -873,6 +963,10 @@
       <c r="G16" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="H16" s="0"/>
+      <c r="I16" s="0"/>
+      <c r="J16" s="0"/>
+      <c r="K16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
@@ -897,6 +991,9 @@
         <v>47</v>
       </c>
       <c r="H17" s="0"/>
+      <c r="I17" s="0"/>
+      <c r="J17" s="0"/>
+      <c r="K17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
@@ -921,6 +1018,9 @@
         <v>50</v>
       </c>
       <c r="H18" s="0"/>
+      <c r="I18" s="0"/>
+      <c r="J18" s="0"/>
+      <c r="K18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
@@ -939,6 +1039,9 @@
       </c>
       <c r="G19" s="0"/>
       <c r="H19" s="0"/>
+      <c r="I19" s="0"/>
+      <c r="J19" s="0"/>
+      <c r="K19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
@@ -957,6 +1060,9 @@
       </c>
       <c r="G20" s="0"/>
       <c r="H20" s="0"/>
+      <c r="I20" s="0"/>
+      <c r="J20" s="0"/>
+      <c r="K20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
@@ -980,6 +1086,10 @@
       <c r="G21" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="H21" s="0"/>
+      <c r="I21" s="0"/>
+      <c r="J21" s="0"/>
+      <c r="K21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
@@ -1006,6 +1116,7 @@
       <c r="H22" s="0"/>
       <c r="I22" s="0"/>
       <c r="J22" s="0"/>
+      <c r="K22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
@@ -1032,6 +1143,7 @@
       <c r="H23" s="0"/>
       <c r="I23" s="0"/>
       <c r="J23" s="0"/>
+      <c r="K23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
@@ -1049,6 +1161,10 @@
         <v>61</v>
       </c>
       <c r="G24" s="0"/>
+      <c r="H24" s="0"/>
+      <c r="I24" s="0"/>
+      <c r="J24" s="0"/>
+      <c r="K24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
@@ -1066,6 +1182,10 @@
         <v>62</v>
       </c>
       <c r="G25" s="0"/>
+      <c r="H25" s="0"/>
+      <c r="I25" s="0"/>
+      <c r="J25" s="0"/>
+      <c r="K25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
@@ -1089,6 +1209,10 @@
       <c r="G26" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="H26" s="0"/>
+      <c r="I26" s="0"/>
+      <c r="J26" s="0"/>
+      <c r="K26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
@@ -1115,6 +1239,7 @@
       <c r="H27" s="0"/>
       <c r="I27" s="0"/>
       <c r="J27" s="0"/>
+      <c r="K27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
@@ -1141,6 +1266,7 @@
       <c r="H28" s="0"/>
       <c r="I28" s="0"/>
       <c r="J28" s="0"/>
+      <c r="K28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
@@ -1158,6 +1284,10 @@
         <v>68</v>
       </c>
       <c r="G29" s="0"/>
+      <c r="H29" s="0"/>
+      <c r="I29" s="0"/>
+      <c r="J29" s="0"/>
+      <c r="K29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
@@ -1175,6 +1305,10 @@
         <v>69</v>
       </c>
       <c r="G30" s="0"/>
+      <c r="H30" s="0"/>
+      <c r="I30" s="0"/>
+      <c r="J30" s="0"/>
+      <c r="K30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="15" t="s">
@@ -1198,6 +1332,10 @@
       <c r="G31" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="H31" s="0"/>
+      <c r="I31" s="0"/>
+      <c r="J31" s="0"/>
+      <c r="K31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="15" t="s">
@@ -1269,6 +1407,9 @@
         <v>75</v>
       </c>
       <c r="G34" s="0"/>
+      <c r="H34" s="0"/>
+      <c r="I34" s="0"/>
+      <c r="J34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="15" t="s">
@@ -1286,6 +1427,9 @@
         <v>-3</v>
       </c>
       <c r="G35" s="0"/>
+      <c r="H35" s="0"/>
+      <c r="I35" s="0"/>
+      <c r="J35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="15" t="s">
@@ -1381,6 +1525,8 @@
         <v>80</v>
       </c>
       <c r="G39" s="0"/>
+      <c r="H39" s="0"/>
+      <c r="I39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="15" t="s">
@@ -1398,172 +1544,382 @@
         <v>81</v>
       </c>
       <c r="G40" s="0"/>
+      <c r="H40" s="0"/>
+      <c r="I40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0"/>
-      <c r="B41" s="0"/>
-      <c r="C41" s="0"/>
-      <c r="D41" s="0"/>
-      <c r="E41" s="0"/>
-      <c r="F41" s="0"/>
-      <c r="G41" s="0"/>
+      <c r="A41" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H41" s="0"/>
+      <c r="I41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="5"/>
+      <c r="B42" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H42" s="0"/>
+      <c r="I42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
-        <v>83</v>
+      <c r="A43" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F43" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G43" s="12" t="s">
+      <c r="G43" s="11"/>
+      <c r="H43" s="0"/>
+      <c r="I43" s="0"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="0"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="11" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>88</v>
       </c>
       <c r="G44" s="0"/>
       <c r="H44" s="0"/>
       <c r="I44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="s">
-        <v>83</v>
+      <c r="A45" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>89</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D45" s="0"/>
+      <c r="E45" s="9"/>
       <c r="F45" s="10" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="G45" s="0"/>
       <c r="H45" s="0"/>
       <c r="I45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="s">
-        <v>83</v>
+      <c r="A46" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G46" s="0"/>
+        <v>11</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="H46" s="0"/>
       <c r="I46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="s">
-        <v>83</v>
+      <c r="A47" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G47" s="0"/>
+        <v>88</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="H47" s="0"/>
       <c r="I47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0"/>
-      <c r="B48" s="0"/>
-      <c r="C48" s="0"/>
-      <c r="D48" s="0"/>
-      <c r="E48" s="0"/>
-      <c r="F48" s="0"/>
-      <c r="G48" s="0"/>
+      <c r="A48" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G48" s="11"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="0"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G49" s="0"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D50" s="0"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G50" s="0"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0"/>
+      <c r="B51" s="0"/>
+      <c r="C51" s="0"/>
+      <c r="D51" s="0"/>
+      <c r="E51" s="0"/>
+      <c r="F51" s="0"/>
+      <c r="G51" s="0"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E49" s="9" t="s">
+      <c r="G53" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="G54" s="0"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G55" s="0"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G56" s="0"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G57" s="0"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0"/>
+      <c r="B58" s="0"/>
+      <c r="C58" s="0"/>
+      <c r="D58" s="0"/>
+      <c r="E58" s="0"/>
+      <c r="F58" s="0"/>
+      <c r="G58" s="0"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E59" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F49" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>86</v>
+      <c r="F59" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated tiny example for memote
</commit_message>
<xml_diff>
--- a/sbmlutils/examples/models/tiny_model/annotations.xlsx
+++ b/sbmlutils/examples/models/tiny_model/annotations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -599,19 +599,18 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F62" activeCellId="0" sqref="F62"/>
+      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="19.5357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.3571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.1632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.4030612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.5357142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="33.5765306122449"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="1" width="19.5357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="19.5357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="20.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.984693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.0255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="34.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="1" width="20.0255102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>